<commit_message>
Task: refactored the test to resolve pylint errors and ran main with inout files with 1000 records or value pairs
</commit_message>
<xml_diff>
--- a/tests/input_excel_files/multiplication_1000values.xlsx
+++ b/tests/input_excel_files/multiplication_1000values.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thulasigovardhan/Documents/NJIT Fall 2021/IS601/csv input files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thulasigovardhan/Desktop/calculator/tests/input_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DFFE70-D60C-9945-91DF-71FBCC09E817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA6C6BD-AA8D-E54D-A8A9-9BAC50117518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{E3D58822-AF80-AC4F-9AB7-178C3CB5323F}"/>
   </bookViews>

</xml_diff>